<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@5e98b418cb53c79ce1ff956206c0de18a2266f33 🚀
</commit_message>
<xml_diff>
--- a/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="292">
   <si>
     <t>Row</t>
   </si>
@@ -738,9 +738,6 @@
   </si>
   <si>
     <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>Rotary_Encoder</t>
   </si>
   <si>
     <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
@@ -1419,7 +1416,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1443,13 +1440,13 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>274</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F2" s="3">
         <v>27</v>
@@ -1457,41 +1454,41 @@
     </row>
     <row r="3" spans="1:22">
       <c r="C3" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>276</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>278</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>280</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1499,13 +1496,13 @@
     </row>
     <row r="6" spans="1:22">
       <c r="C6" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>282</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F6" s="3">
         <v>58</v>
@@ -3166,7 +3163,7 @@
         <v>239</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>240</v>
+        <v>63</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>22</v>
@@ -3178,7 +3175,7 @@
         <v>31</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M32" s="10" t="s">
         <v>33</v>
@@ -3187,10 +3184,10 @@
         <v>51</v>
       </c>
       <c r="O32" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="P32" s="10" t="s">
         <v>242</v>
-      </c>
-      <c r="P32" s="10" t="s">
-        <v>243</v>
       </c>
       <c r="Q32" s="10" t="s">
         <v>37</v>
@@ -3205,15 +3202,15 @@
         <v>40</v>
       </c>
       <c r="U32" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="V32" s="10" t="s">
         <v>244</v>
-      </c>
-      <c r="V32" s="10" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>235</v>
@@ -3225,16 +3222,16 @@
         <v>25</v>
       </c>
       <c r="E33" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>247</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>248</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>239</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>240</v>
+        <v>63</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>22</v>
@@ -3246,7 +3243,7 @@
         <v>31</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M33" s="7" t="s">
         <v>33</v>
@@ -3255,10 +3252,10 @@
         <v>51</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Q33" s="7" t="s">
         <v>37</v>
@@ -3273,36 +3270,36 @@
         <v>40</v>
       </c>
       <c r="U33" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="V33" s="7" t="s">
         <v>244</v>
-      </c>
-      <c r="V33" s="7" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="C34" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="F34" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="G34" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="F34" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="G34" s="10" t="s">
+      <c r="H34" s="10" t="s">
         <v>255</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>256</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>22</v>
@@ -3314,7 +3311,7 @@
         <v>31</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M34" s="10" t="s">
         <v>33</v>
@@ -3323,10 +3320,10 @@
         <v>51</v>
       </c>
       <c r="O34" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="P34" s="10" t="s">
         <v>258</v>
-      </c>
-      <c r="P34" s="10" t="s">
-        <v>259</v>
       </c>
       <c r="Q34" s="10" t="s">
         <v>95</v>
@@ -3341,33 +3338,33 @@
         <v>40</v>
       </c>
       <c r="U34" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="V34" s="10" t="s">
         <v>260</v>
-      </c>
-      <c r="V34" s="10" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="C35" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="E35" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="F35" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="G35" s="7" t="s">
         <v>266</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>267</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>63</v>
@@ -3382,7 +3379,7 @@
         <v>31</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="M35" s="7" t="s">
         <v>33</v>
@@ -3391,10 +3388,10 @@
         <v>51</v>
       </c>
       <c r="O35" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="P35" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="P35" s="7" t="s">
-        <v>270</v>
       </c>
       <c r="Q35" s="7" t="s">
         <v>54</v>
@@ -3409,7 +3406,7 @@
         <v>40</v>
       </c>
       <c r="U35" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="V35" s="7" t="s">
         <v>161</v>
@@ -3438,22 +3435,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@107eaa5d8d474005d9574e15f9211dfb57529940 🚀
</commit_message>
<xml_diff>
--- a/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="299">
   <si>
     <t>Row</t>
   </si>
@@ -569,6 +569,30 @@
     <t>14</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>PDQE15-Q24-S5-D</t>
+  </si>
+  <si>
+    <t>PS1</t>
+  </si>
+  <si>
+    <t>CONV_PDQE15-Q24-S5-D</t>
+  </si>
+  <si>
+    <t>/psu</t>
+  </si>
+  <si>
+    <t>-20.0000</t>
+  </si>
+  <si>
+    <t>125.0000</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>Resistor</t>
   </si>
   <si>
@@ -593,7 +617,7 @@
     <t>55.6600</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
   <si>
     <t>R3</t>
@@ -608,7 +632,7 @@
     <t>61.9500</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
   <si>
     <t>R1</t>
@@ -623,7 +647,7 @@
     <t>56.0200</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
   <si>
     <t>R2 R5</t>
@@ -635,7 +659,7 @@
     <t>58.9500</t>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
   <si>
     <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
@@ -671,7 +695,7 @@
     <t>7.5000</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>SW5</t>
@@ -683,7 +707,7 @@
     <t>78.7500</t>
   </si>
   <si>
-    <t>20</t>
+    <t>21</t>
   </si>
   <si>
     <t>SW6</t>
@@ -692,7 +716,7 @@
     <t>153.7500</t>
   </si>
   <si>
-    <t>21</t>
+    <t>22</t>
   </si>
   <si>
     <t>SW1</t>
@@ -704,7 +728,7 @@
     <t>60.5000</t>
   </si>
   <si>
-    <t>22</t>
+    <t>23</t>
   </si>
   <si>
     <t>SW2</t>
@@ -713,7 +737,7 @@
     <t>E</t>
   </si>
   <si>
-    <t>23</t>
+    <t>24</t>
   </si>
   <si>
     <t>SW3</t>
@@ -722,7 +746,7 @@
     <t>F</t>
   </si>
   <si>
-    <t>24</t>
+    <t>25</t>
   </si>
   <si>
     <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
@@ -755,7 +779,7 @@
     <t>14.4000</t>
   </si>
   <si>
-    <t>25</t>
+    <t>26</t>
   </si>
   <si>
     <t>SW7</t>
@@ -767,7 +791,7 @@
     <t>40.2500</t>
   </si>
   <si>
-    <t>26</t>
+    <t>27</t>
   </si>
   <si>
     <t>Schmitt Trigger Output Optocoupler, High Speed, DIP-6, 1.6mA turn on threshold</t>
@@ -803,10 +827,7 @@
     <t>6.6800</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t/>
+    <t>28</t>
   </si>
   <si>
     <t>Pico</t>
@@ -872,7 +893,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>58 (0 SMD/ 56 THT)</t>
+    <t>59 (0 SMD/ 56 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -932,7 +953,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -983,6 +1004,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF8A8A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF8080"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1000,7 +1027,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1033,6 +1060,9 @@
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1381,7 +1411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1395,7 +1425,7 @@
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" customWidth="1"/>
     <col min="5" max="5" width="43.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="60.7109375" customWidth="1"/>
     <col min="8" max="8" width="31.7109375" customWidth="1"/>
     <col min="9" max="9" width="26.7109375" customWidth="1"/>
@@ -1416,7 +1446,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1440,55 +1470,55 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" s="2" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="F2" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="C3" s="2" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="2" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="2" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1496,16 +1526,16 @@
     </row>
     <row r="6" spans="1:22">
       <c r="C6" s="2" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="F6" s="3">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -2464,26 +2494,26 @@
       <c r="A22" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="11" t="s">
         <v>183</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>184</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>25</v>
+        <v>184</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>185</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>64</v>
+        <v>184</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="H22" s="10" t="s">
-        <v>187</v>
+      <c r="H22" s="11" t="s">
+        <v>183</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>22</v>
@@ -2494,20 +2524,20 @@
       <c r="K22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L22" s="10" t="s">
-        <v>188</v>
+      <c r="L22" s="11" t="s">
+        <v>183</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>33</v>
+        <v>187</v>
       </c>
       <c r="N22" s="8" t="s">
         <v>51</v>
       </c>
       <c r="O22" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="P22" s="10" t="s">
         <v>189</v>
-      </c>
-      <c r="P22" s="10" t="s">
-        <v>190</v>
       </c>
       <c r="Q22" s="10" t="s">
         <v>37</v>
@@ -2516,42 +2546,42 @@
         <v>38</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
       <c r="T22" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U22" s="10" t="s">
-        <v>181</v>
+        <v>37</v>
       </c>
       <c r="V22" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>183</v>
-      </c>
       <c r="C23" s="7" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>193</v>
+        <v>64</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>22</v>
@@ -2563,7 +2593,7 @@
         <v>31</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="M23" s="7" t="s">
         <v>33</v>
@@ -2572,10 +2602,10 @@
         <v>51</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="Q23" s="7" t="s">
         <v>37</v>
@@ -2598,28 +2628,28 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="8" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>22</v>
@@ -2631,7 +2661,7 @@
         <v>31</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="M24" s="10" t="s">
         <v>33</v>
@@ -2640,13 +2670,13 @@
         <v>51</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="Q24" s="10" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="R24" s="10" t="s">
         <v>38</v>
@@ -2666,55 +2696,55 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="K25" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="M25" s="7" t="s">
         <v>33</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>119</v>
+        <v>51</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="Q25" s="7" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="R25" s="7" t="s">
         <v>38</v>
@@ -2732,54 +2762,54 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="30" customHeight="1">
+    <row r="26" spans="1:22">
       <c r="A26" s="8" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>208</v>
+        <v>25</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>63</v>
+        <v>195</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="M26" s="10" t="s">
         <v>33</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="Q26" s="10" t="s">
         <v>37</v>
@@ -2794,33 +2824,33 @@
         <v>40</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
       <c r="V26" s="10" t="s">
-        <v>216</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>219</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>63</v>
@@ -2835,7 +2865,7 @@
         <v>31</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="M27" s="7" t="s">
         <v>33</v>
@@ -2844,10 +2874,10 @@
         <v>51</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="Q27" s="7" t="s">
         <v>37</v>
@@ -2862,33 +2892,33 @@
         <v>40</v>
       </c>
       <c r="U27" s="7" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="V27" s="7" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="30" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>24</v>
+        <v>227</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="H28" s="10" t="s">
         <v>63</v>
@@ -2903,7 +2933,7 @@
         <v>31</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="M28" s="10" t="s">
         <v>33</v>
@@ -2912,10 +2942,10 @@
         <v>51</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="P28" s="10" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="Q28" s="10" t="s">
         <v>37</v>
@@ -2930,33 +2960,33 @@
         <v>40</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="V28" s="10" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>226</v>
+        <v>24</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>63</v>
@@ -2971,7 +3001,7 @@
         <v>31</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="M29" s="7" t="s">
         <v>33</v>
@@ -2980,10 +3010,10 @@
         <v>51</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="P29" s="7" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="Q29" s="7" t="s">
         <v>37</v>
@@ -2998,33 +3028,33 @@
         <v>40</v>
       </c>
       <c r="U29" s="7" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="V29" s="7" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="30" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="H30" s="10" t="s">
         <v>63</v>
@@ -3039,7 +3069,7 @@
         <v>31</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="M30" s="10" t="s">
         <v>33</v>
@@ -3048,10 +3078,10 @@
         <v>51</v>
       </c>
       <c r="O30" s="10" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="P30" s="10" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="Q30" s="10" t="s">
         <v>37</v>
@@ -3066,33 +3096,33 @@
         <v>40</v>
       </c>
       <c r="U30" s="10" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="V30" s="10" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>63</v>
@@ -3107,7 +3137,7 @@
         <v>31</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="M31" s="7" t="s">
         <v>33</v>
@@ -3116,10 +3146,10 @@
         <v>51</v>
       </c>
       <c r="O31" s="7" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="Q31" s="7" t="s">
         <v>37</v>
@@ -3134,33 +3164,33 @@
         <v>40</v>
       </c>
       <c r="U31" s="7" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="30" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>25</v>
+        <v>216</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="H32" s="10" t="s">
         <v>63</v>
@@ -3175,7 +3205,7 @@
         <v>31</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="M32" s="10" t="s">
         <v>33</v>
@@ -3184,10 +3214,10 @@
         <v>51</v>
       </c>
       <c r="O32" s="10" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="P32" s="10" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="Q32" s="10" t="s">
         <v>37</v>
@@ -3202,33 +3232,33 @@
         <v>40</v>
       </c>
       <c r="U32" s="10" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="V32" s="10" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E33" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="G33" s="7" t="s">
         <v>247</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>239</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>63</v>
@@ -3243,7 +3273,7 @@
         <v>31</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="M33" s="7" t="s">
         <v>33</v>
@@ -3252,10 +3282,10 @@
         <v>51</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="Q33" s="7" t="s">
         <v>37</v>
@@ -3270,36 +3300,36 @@
         <v>40</v>
       </c>
       <c r="U33" s="7" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>252</v>
+        <v>25</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>255</v>
+        <v>63</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>22</v>
@@ -3311,7 +3341,7 @@
         <v>31</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="M34" s="10" t="s">
         <v>33</v>
@@ -3320,13 +3350,13 @@
         <v>51</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="P34" s="10" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="Q34" s="10" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="R34" s="10" t="s">
         <v>38</v>
@@ -3338,36 +3368,36 @@
         <v>40</v>
       </c>
       <c r="U34" s="10" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="V34" s="10" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="F35" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="G35" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="H35" s="7" t="s">
         <v>263</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>22</v>
@@ -3379,7 +3409,7 @@
         <v>31</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="M35" s="7" t="s">
         <v>33</v>
@@ -3388,16 +3418,16 @@
         <v>51</v>
       </c>
       <c r="O35" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="P35" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="Q35" s="7" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="R35" s="7" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="S35" s="7" t="s">
         <v>39</v>
@@ -3406,9 +3436,77 @@
         <v>40</v>
       </c>
       <c r="U35" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="V35" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="30" customHeight="1">
+      <c r="A36" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="V35" s="7" t="s">
+      <c r="D36" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L36" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="M36" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N36" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="O36" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="P36" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q36" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="R36" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="S36" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="T36" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="U36" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="V36" s="10" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3435,22 +3533,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="11" t="s">
-        <v>291</v>
+      <c r="A4" s="12" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@5e87075115d2cf433a2bd3a43b39d9bc4ae52a4b 🚀
</commit_message>
<xml_diff>
--- a/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="337">
   <si>
     <t>Row</t>
   </si>
@@ -98,6 +98,51 @@
     <t>Device</t>
   </si>
   <si>
+    <t>C18 C19</t>
+  </si>
+  <si>
+    <t>1nF</t>
+  </si>
+  <si>
+    <t>C_Disc_D7.5mm_W4.4mm_P5.00mm</t>
+  </si>
+  <si>
+    <t>Capacitor_THT</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://connect.kemet.com:7667/gateway/IntelliData-ComponentDocumentation/1.0/download/datasheet/C322C101K1G5TA7301.pdf</t>
+  </si>
+  <si>
+    <t>/psu</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(2)</t>
+  </si>
+  <si>
+    <t>-20.0000</t>
+  </si>
+  <si>
+    <t>125.0000</t>
+  </si>
+  <si>
+    <t>0.0000</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
     <t>C1 C2 C3 C4 C5 C6 C7 C8 C9 C10 C11 C12</t>
   </si>
   <si>
@@ -107,15 +152,9 @@
     <t>C_Disc_D3.0mm_W1.6mm_P2.50mm</t>
   </si>
   <si>
-    <t>Capacitor_THT</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>https://www.vishay.com/docs/45171/kseries.pdf</t>
   </si>
   <si>
@@ -131,25 +170,55 @@
     <t>81.3000</t>
   </si>
   <si>
-    <t>0.0000</t>
-  </si>
-  <si>
-    <t>top</t>
-  </si>
-  <si>
     <t>THT</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>4.1000</t>
   </si>
   <si>
     <t>1.6000</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>C16 C17</t>
+  </si>
+  <si>
+    <t>4.7uF 50V</t>
+  </si>
+  <si>
+    <t>C_Disc_D5.1mm_W3.2mm_P5.00mm</t>
+  </si>
+  <si>
+    <t>https://connect.kemet.com:7667/gateway/IntelliData-ComponentDocumentation/1.0/download/datasheet/C322C102K1R5TA.pdf</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Polarized capacitor</t>
+  </si>
+  <si>
+    <t>C_Polarized</t>
+  </si>
+  <si>
+    <t>C13 C14 C15</t>
+  </si>
+  <si>
+    <t>220uF</t>
+  </si>
+  <si>
+    <t>CP_Radial_D10.0mm_P5.00mm</t>
+  </si>
+  <si>
+    <t>https://www.cde.com/resources/catalogs/AVG.pdf</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(3)</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <t>100V 0.15A standard switching diode, DO-35</t>
@@ -188,7 +257,7 @@
     <t>9.2200</t>
   </si>
   <si>
-    <t>3</t>
+    <t>6</t>
   </si>
   <si>
     <t>RGB LED with integrated controller, 5mm/8mm LED package</t>
@@ -233,7 +302,49 @@
     <t>1.8000</t>
   </si>
   <si>
-    <t>4</t>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Resettable fuse, polymeric positive temperature coefficient</t>
+  </si>
+  <si>
+    <t>Polyfuse</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>DC Barrel Jack with a mounting pin</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_MountingPin</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>BarrelJack_CUI_PJ-063AH_Horizontal</t>
+  </si>
+  <si>
+    <t>Connector_BarrelJack</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/pj-063ah.pdf</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
   <si>
     <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
@@ -254,9 +365,6 @@
     <t>Jack_6.35mm_Horizontal</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
   </si>
   <si>
@@ -281,9 +389,6 @@
     <t>Raspberry_Pi_2_3</t>
   </si>
   <si>
-    <t>Connector</t>
-  </si>
-  <si>
     <t>J8</t>
   </si>
   <si>
@@ -317,7 +422,7 @@
     <t>55.0150</t>
   </si>
   <si>
-    <t>6</t>
+    <t>11</t>
   </si>
   <si>
     <t>Generic connector, double row, 02x03, top/bottom pin numbering scheme (row 1: 1...pins_per_row, row2: pins_per_row+1 ... num_pins), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
@@ -356,9 +461,6 @@
     <t>6.7800</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
   </si>
   <si>
@@ -377,9 +479,6 @@
     <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
   </si>
   <si>
-    <t>pedalboard-hw(2)</t>
-  </si>
-  <si>
     <t>96.0000</t>
   </si>
   <si>
@@ -392,7 +491,7 @@
     <t>6.7000</t>
   </si>
   <si>
-    <t>8</t>
+    <t>13</t>
   </si>
   <si>
     <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
@@ -416,16 +515,13 @@
     <t>103.0000</t>
   </si>
   <si>
-    <t>SMD</t>
-  </si>
-  <si>
     <t>17.5000</t>
   </si>
   <si>
     <t>14.7500</t>
   </si>
   <si>
-    <t>9</t>
+    <t>14</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x02, script generated</t>
@@ -455,6 +551,9 @@
     <t>3.3500</t>
   </si>
   <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>Generic connector, single row, 01x03, script generated</t>
   </si>
   <si>
@@ -482,7 +581,7 @@
     <t>1.7000</t>
   </si>
   <si>
-    <t>11</t>
+    <t>16</t>
   </si>
   <si>
     <t>J7</t>
@@ -506,6 +605,9 @@
     <t>49.9600</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
     <t>USB Type A connector</t>
   </si>
   <si>
@@ -530,7 +632,22 @@
     <t>9.3200</t>
   </si>
   <si>
-    <t>13</t>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>2.2uH</t>
+  </si>
+  <si>
+    <t>19</t>
   </si>
   <si>
     <t>Inductor with ferrite core</t>
@@ -566,10 +683,7 @@
     <t>11.7600</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t/>
+    <t>20</t>
   </si>
   <si>
     <t>PDQE15-Q24-S5-D</t>
@@ -581,16 +695,19 @@
     <t>CONV_PDQE15-Q24-S5-D</t>
   </si>
   <si>
-    <t>/psu</t>
-  </si>
-  <si>
-    <t>-20.0000</t>
-  </si>
-  <si>
-    <t>125.0000</t>
-  </si>
-  <si>
-    <t>15</t>
+    <t>https://www.cui.com/product/resource/pdqe15-d.pdf</t>
+  </si>
+  <si>
+    <t>114.9000</t>
+  </si>
+  <si>
+    <t>49.8000</t>
+  </si>
+  <si>
+    <t>22.5700</t>
+  </si>
+  <si>
+    <t>21</t>
   </si>
   <si>
     <t>Resistor</t>
@@ -617,7 +734,7 @@
     <t>55.6600</t>
   </si>
   <si>
-    <t>16</t>
+    <t>22</t>
   </si>
   <si>
     <t>R3</t>
@@ -632,7 +749,7 @@
     <t>61.9500</t>
   </si>
   <si>
-    <t>17</t>
+    <t>23</t>
   </si>
   <si>
     <t>R1</t>
@@ -647,7 +764,7 @@
     <t>56.0200</t>
   </si>
   <si>
-    <t>18</t>
+    <t>24</t>
   </si>
   <si>
     <t>R2 R5</t>
@@ -659,7 +776,7 @@
     <t>58.9500</t>
   </si>
   <si>
-    <t>19</t>
+    <t>25</t>
   </si>
   <si>
     <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
@@ -695,7 +812,7 @@
     <t>7.5000</t>
   </si>
   <si>
-    <t>20</t>
+    <t>26</t>
   </si>
   <si>
     <t>SW5</t>
@@ -707,7 +824,7 @@
     <t>78.7500</t>
   </si>
   <si>
-    <t>21</t>
+    <t>27</t>
   </si>
   <si>
     <t>SW6</t>
@@ -716,7 +833,7 @@
     <t>153.7500</t>
   </si>
   <si>
-    <t>22</t>
+    <t>28</t>
   </si>
   <si>
     <t>SW1</t>
@@ -728,7 +845,7 @@
     <t>60.5000</t>
   </si>
   <si>
-    <t>23</t>
+    <t>29</t>
   </si>
   <si>
     <t>SW2</t>
@@ -737,7 +854,7 @@
     <t>E</t>
   </si>
   <si>
-    <t>24</t>
+    <t>30</t>
   </si>
   <si>
     <t>SW3</t>
@@ -746,7 +863,7 @@
     <t>F</t>
   </si>
   <si>
-    <t>25</t>
+    <t>31</t>
   </si>
   <si>
     <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
@@ -779,7 +896,7 @@
     <t>14.4000</t>
   </si>
   <si>
-    <t>26</t>
+    <t>32</t>
   </si>
   <si>
     <t>SW7</t>
@@ -791,9 +908,6 @@
     <t>40.2500</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>Schmitt Trigger Output Optocoupler, High Speed, DIP-6, 1.6mA turn on threshold</t>
   </si>
   <si>
@@ -827,7 +941,7 @@
     <t>6.6800</t>
   </si>
   <si>
-    <t>28</t>
+    <t>34</t>
   </si>
   <si>
     <t>Pico</t>
@@ -893,7 +1007,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>59 (0 SMD/ 56 THT)</t>
+    <t>69 (0 SMD/ 57 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -1004,13 +1118,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8A8A"/>
+        <fgColor rgb="FFFF8080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8080"/>
+        <fgColor rgb="FFFF8A8A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1411,7 +1525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V36"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1422,10 +1536,10 @@
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" customWidth="1"/>
     <col min="5" max="5" width="43.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" customWidth="1"/>
     <col min="7" max="7" width="60.7109375" customWidth="1"/>
     <col min="8" max="8" width="31.7109375" customWidth="1"/>
     <col min="9" max="9" width="26.7109375" customWidth="1"/>
@@ -1446,7 +1560,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>278</v>
+        <v>316</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1470,55 +1584,55 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" s="2" t="s">
-        <v>279</v>
+        <v>317</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>280</v>
+        <v>318</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>289</v>
+        <v>327</v>
       </c>
       <c r="F2" s="3">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="C3" s="2" t="s">
-        <v>281</v>
+        <v>319</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>290</v>
+        <v>328</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>291</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="2" t="s">
-        <v>283</v>
+        <v>321</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>284</v>
+        <v>322</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>292</v>
+        <v>330</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>291</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="2" t="s">
-        <v>285</v>
+        <v>323</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>286</v>
+        <v>324</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>293</v>
+        <v>331</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1526,16 +1640,16 @@
     </row>
     <row r="6" spans="1:22">
       <c r="C6" s="2" t="s">
-        <v>287</v>
+        <v>325</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>288</v>
+        <v>326</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>294</v>
+        <v>332</v>
       </c>
       <c r="F6" s="3">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -1606,7 +1720,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1668,128 +1782,128 @@
         <v>40</v>
       </c>
       <c r="U9" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="V9" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="H10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="J10" s="8" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="Q10" s="10" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="R10" s="10" t="s">
         <v>38</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T10" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="V10" s="10" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>62</v>
-      </c>
       <c r="H11" s="7" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="M11" s="7" t="s">
         <v>33</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="Q11" s="7" t="s">
         <v>37</v>
@@ -1804,60 +1918,60 @@
         <v>40</v>
       </c>
       <c r="U11" s="7" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="30" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="8" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="M12" s="10" t="s">
         <v>33</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="O12" s="10" t="s">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="Q12" s="10" t="s">
         <v>37</v>
@@ -1872,36 +1986,36 @@
         <v>40</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="V12" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="30" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="5" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>22</v>
@@ -1913,158 +2027,158 @@
         <v>31</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="R13" s="7" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T13" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="60" customHeight="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="30" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="R14" s="10" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T14" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="V14" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="30" customHeight="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="5" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>63</v>
+        <v>96</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="K15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="7" t="s">
-        <v>118</v>
+      <c r="L15" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="M15" s="7" t="s">
         <v>33</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>120</v>
+        <v>35</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>121</v>
+        <v>36</v>
       </c>
       <c r="Q15" s="7" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="R15" s="7" t="s">
         <v>38</v>
@@ -2076,172 +2190,172 @@
         <v>40</v>
       </c>
       <c r="U15" s="7" t="s">
-        <v>122</v>
+        <v>37</v>
       </c>
       <c r="V15" s="7" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="8" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="M16" s="10" t="s">
         <v>33</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>120</v>
+        <v>35</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>131</v>
+        <v>36</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="R16" s="10" t="s">
         <v>38</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>132</v>
+        <v>39</v>
       </c>
       <c r="T16" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>133</v>
+        <v>37</v>
       </c>
       <c r="V16" s="10" t="s">
-        <v>134</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="R17" s="7" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="S17" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T17" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U17" s="7" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="30" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>22</v>
@@ -2253,63 +2367,63 @@
         <v>31</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="Q18" s="10" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="R18" s="10" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T18" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="V18" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="60" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>63</v>
+        <v>141</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>22</v>
@@ -2321,158 +2435,158 @@
         <v>31</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="Q19" s="7" t="s">
-        <v>54</v>
+        <v>130</v>
       </c>
       <c r="R19" s="7" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T19" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U19" s="7" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="V19" s="7" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="30" customHeight="1">
       <c r="A20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="J20" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="Q20" s="10" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T20" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="V20" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="30" customHeight="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" s="5" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>176</v>
+        <v>86</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="O21" s="7" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="R21" s="7" t="s">
         <v>38</v>
@@ -2484,36 +2598,36 @@
         <v>40</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>183</v>
+        <v>167</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>184</v>
+        <v>103</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>183</v>
+        <v>172</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>22</v>
@@ -2524,64 +2638,64 @@
       <c r="K22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L22" s="11" t="s">
-        <v>183</v>
+      <c r="L22" s="10" t="s">
+        <v>173</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>187</v>
+        <v>46</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="P22" s="10" t="s">
-        <v>189</v>
+        <v>91</v>
       </c>
       <c r="Q22" s="10" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="R22" s="10" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>132</v>
+        <v>50</v>
       </c>
       <c r="T22" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U22" s="10" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
       <c r="V22" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>64</v>
+        <v>181</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>195</v>
+        <v>141</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>22</v>
@@ -2593,63 +2707,63 @@
         <v>31</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="Q23" s="7" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T23" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U23" s="7" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="V23" s="7" t="s">
-        <v>42</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="8" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>191</v>
+        <v>121</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>192</v>
+        <v>122</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>195</v>
+        <v>86</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>22</v>
@@ -2661,63 +2775,63 @@
         <v>31</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="Q24" s="10" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="R24" s="10" t="s">
         <v>38</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T24" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U24" s="10" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="V24" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>195</v>
+        <v>86</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>22</v>
@@ -2729,87 +2843,87 @@
         <v>31</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="Q25" s="7" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="R25" s="7" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="S25" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T25" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U25" s="7" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>42</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>195</v>
+        <v>208</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L26" s="10" t="s">
-        <v>196</v>
+      <c r="L26" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="M26" s="10" t="s">
         <v>33</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>202</v>
+        <v>35</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>212</v>
+        <v>36</v>
       </c>
       <c r="Q26" s="10" t="s">
         <v>37</v>
@@ -2824,104 +2938,104 @@
         <v>40</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>181</v>
+        <v>37</v>
       </c>
       <c r="V26" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="F27" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="G27" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="H27" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="I27" s="5" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="Q27" s="7" t="s">
-        <v>37</v>
+        <v>219</v>
       </c>
       <c r="R27" s="7" t="s">
         <v>38</v>
       </c>
       <c r="S27" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T27" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U27" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="V27" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22">
+      <c r="A28" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="E28" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="V27" s="7" t="s">
+      <c r="F28" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" ht="30" customHeight="1">
-      <c r="A28" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>63</v>
+      <c r="H28" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>22</v>
@@ -2933,63 +3047,63 @@
         <v>31</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="M28" s="10" t="s">
         <v>33</v>
       </c>
       <c r="N28" s="8" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="P28" s="10" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="Q28" s="10" t="s">
-        <v>37</v>
+        <v>219</v>
       </c>
       <c r="R28" s="10" t="s">
         <v>38</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T28" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="V28" s="10" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" ht="30" customHeight="1">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" s="5" t="s">
         <v>229</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>216</v>
+        <v>25</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>63</v>
+        <v>234</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>22</v>
@@ -3001,19 +3115,19 @@
         <v>31</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="P29" s="7" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="Q29" s="7" t="s">
         <v>37</v>
@@ -3022,42 +3136,42 @@
         <v>38</v>
       </c>
       <c r="S29" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T29" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U29" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="V29" s="7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" ht="30" customHeight="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30" s="8" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>216</v>
+        <v>25</v>
       </c>
       <c r="E30" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="G30" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="H30" s="10" t="s">
         <v>234</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>63</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>22</v>
@@ -3069,19 +3183,19 @@
         <v>31</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="M30" s="10" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O30" s="10" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="P30" s="10" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="Q30" s="10" t="s">
         <v>37</v>
@@ -3090,42 +3204,42 @@
         <v>38</v>
       </c>
       <c r="S30" s="10" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T30" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U30" s="10" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="V30" s="10" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="30" customHeight="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22">
       <c r="A31" s="5" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>216</v>
+        <v>25</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>63</v>
+        <v>234</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>22</v>
@@ -3137,87 +3251,87 @@
         <v>31</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="M31" s="7" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O31" s="7" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="Q31" s="7" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="R31" s="7" t="s">
         <v>38</v>
       </c>
       <c r="S31" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T31" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U31" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" ht="30" customHeight="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22">
       <c r="A32" s="8" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>216</v>
+        <v>25</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>63</v>
+        <v>234</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="K32" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="M32" s="10" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="O32" s="10" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="P32" s="10" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="Q32" s="10" t="s">
         <v>37</v>
@@ -3226,42 +3340,42 @@
         <v>38</v>
       </c>
       <c r="S32" s="10" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T32" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U32" s="10" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="V32" s="10" t="s">
-        <v>224</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>25</v>
+        <v>255</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>22</v>
@@ -3273,19 +3387,19 @@
         <v>31</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="M33" s="7" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="Q33" s="7" t="s">
         <v>37</v>
@@ -3294,42 +3408,42 @@
         <v>38</v>
       </c>
       <c r="S33" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T33" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U33" s="7" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>243</v>
-      </c>
       <c r="C34" s="10" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>25</v>
+        <v>255</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>22</v>
@@ -3341,19 +3455,19 @@
         <v>31</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="M34" s="10" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="P34" s="10" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="Q34" s="10" t="s">
         <v>37</v>
@@ -3362,42 +3476,42 @@
         <v>38</v>
       </c>
       <c r="S34" s="10" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T34" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U34" s="10" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="V34" s="10" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>262</v>
-      </c>
       <c r="H35" s="7" t="s">
-        <v>263</v>
+        <v>86</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>22</v>
@@ -3409,63 +3523,63 @@
         <v>31</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="M35" s="7" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O35" s="7" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="P35" s="7" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="Q35" s="7" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="R35" s="7" t="s">
         <v>38</v>
       </c>
       <c r="S35" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T35" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U35" s="7" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="V35" s="7" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>183</v>
+        <v>271</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>253</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="E36" s="10" t="s">
         <v>272</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>22</v>
@@ -3477,37 +3591,445 @@
         <v>31</v>
       </c>
       <c r="L36" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="M36" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="N36" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="O36" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="P36" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="M36" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="N36" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="O36" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="P36" s="10" t="s">
-        <v>276</v>
-      </c>
       <c r="Q36" s="10" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="R36" s="10" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="S36" s="10" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T36" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U36" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="V36" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" ht="30" customHeight="1">
+      <c r="A37" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="V36" s="10" t="s">
-        <v>161</v>
+      <c r="G37" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N37" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O37" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="P37" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q37" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="R37" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="S37" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="T37" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="U37" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="V37" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" ht="30" customHeight="1">
+      <c r="A38" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L38" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="M38" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="N38" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="O38" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="P38" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q38" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="R38" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="S38" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="T38" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="U38" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="V38" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" ht="30" customHeight="1">
+      <c r="A39" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="M39" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O39" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="P39" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q39" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="R39" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="S39" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="T39" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="U39" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="V39" s="7" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="30" customHeight="1">
+      <c r="A40" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L40" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="M40" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="N40" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="O40" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="P40" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q40" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="R40" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="S40" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="T40" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="U40" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="V40" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" ht="30" customHeight="1">
+      <c r="A41" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N41" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O41" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="P41" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q41" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="R41" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="S41" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="T41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="U41" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="V41" s="7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" ht="30" customHeight="1">
+      <c r="A42" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K42" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L42" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="M42" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="N42" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="O42" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q42" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="R42" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="S42" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="T42" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="U42" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="V42" s="10" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -3533,22 +4055,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>295</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>296</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>297</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="12" t="s">
-        <v>298</v>
+      <c r="A4" s="11" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@4e9427fa4a93b9db6b68d88efed63e44f57f6ac2 🚀
</commit_message>
<xml_diff>
--- a/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -692,7 +692,7 @@
     <t>93.6250</t>
   </si>
   <si>
-    <t>35.0150</t>
+    <t>27.2200</t>
   </si>
   <si>
     <t>9.3200</t>
@@ -3001,7 +3001,7 @@
         <v>224</v>
       </c>
       <c r="Q26" s="10" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="R26" s="10" t="s">
         <v>132</v>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@6d01424e469efda87abd38c5be86be76e11475e6 🚀
</commit_message>
<xml_diff>
--- a/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -704,10 +704,10 @@
     <t>https://www.we-online.com/components/products/datasheet/6130xx11021.pdf</t>
   </si>
   <si>
-    <t>23.6150</t>
-  </si>
-  <si>
-    <t>42.2100</t>
+    <t>35.8650</t>
+  </si>
+  <si>
+    <t>42.0374</t>
   </si>
   <si>
     <t>19</t>
@@ -3061,7 +3061,7 @@
         <v>229</v>
       </c>
       <c r="Q26" s="10" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="R26" s="10" t="s">
         <v>152</v>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@5949c402c5f4cc4ae07c4ac612c1f53ef18ab881 🚀
</commit_message>
<xml_diff>
--- a/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -227,7 +227,7 @@
     <t>pedalboard-hw(3)</t>
   </si>
   <si>
-    <t>138.5699</t>
+    <t>140.5323</t>
   </si>
   <si>
     <t>87.5000</t>
@@ -296,10 +296,10 @@
     <t>http://www.vishay.com/docs/88516/1n5400.pdf</t>
   </si>
   <si>
-    <t>135.1940</t>
-  </si>
-  <si>
-    <t>96.1964</t>
+    <t>134.7000</t>
+  </si>
+  <si>
+    <t>79.1000</t>
   </si>
   <si>
     <t>18.4400</t>
@@ -407,10 +407,10 @@
     <t>https://www.onsemi.com/pdf/datasheet/1n5400-d.pdf</t>
   </si>
   <si>
-    <t>142.0012</t>
-  </si>
-  <si>
-    <t>101.2256</t>
+    <t>151.9000</t>
+  </si>
+  <si>
+    <t>95.2000</t>
   </si>
   <si>
     <t>DC Barrel Jack with an internal switch</t>
@@ -2245,7 +2245,7 @@
         <v>93</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="R14" s="10" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@0fd8c3d01bfd357797580081104765e6a05b3b07 🚀
</commit_message>
<xml_diff>
--- a/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="420">
   <si>
     <t>Row</t>
   </si>
@@ -1111,6 +1111,33 @@
     <t>38</t>
   </si>
   <si>
+    <t>OR Gate IC 1 Channel - SOT-353</t>
+  </si>
+  <si>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>SOT-353_SC-70-5</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD</t>
+  </si>
+  <si>
+    <t>52.9500</t>
+  </si>
+  <si>
+    <t>77.9500</t>
+  </si>
+  <si>
+    <t>2.5500</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
     <t>Schmitt Trigger Output Optocoupler, High Speed, DIP-6, 1.6mA turn on threshold</t>
   </si>
   <si>
@@ -1144,7 +1171,7 @@
     <t>6.6800</t>
   </si>
   <si>
-    <t>39</t>
+    <t>40</t>
   </si>
   <si>
     <t>Pico</t>
@@ -1210,13 +1237,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>82 (4 SMD/ 76 THT)</t>
+    <t>83 (5 SMD/ 76 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>76 (4 SMD/ 70 THT)</t>
+    <t>77 (5 SMD/ 70 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -1801,7 +1828,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V47"/>
+  <dimension ref="A1:V48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1836,7 +1863,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1860,55 +1887,55 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" s="2" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="F2" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="C3" s="2" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="2" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="2" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1916,16 +1943,16 @@
     </row>
     <row r="6" spans="1:22">
       <c r="C6" s="2" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="F6" s="3">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -4512,7 +4539,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="30" customHeight="1">
+    <row r="46" spans="1:22">
       <c r="A46" s="8" t="s">
         <v>362</v>
       </c>
@@ -4523,19 +4550,19 @@
         <v>364</v>
       </c>
       <c r="D46" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="E46" s="10" t="s">
         <v>365</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>366</v>
       </c>
       <c r="F46" s="10" t="s">
         <v>364</v>
       </c>
       <c r="G46" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="H46" s="10" t="s">
         <v>367</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>368</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>22</v>
@@ -4546,20 +4573,20 @@
       <c r="K46" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L46" s="10" t="s">
-        <v>369</v>
+      <c r="L46" s="11" t="s">
+        <v>288</v>
       </c>
       <c r="M46" s="10" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="N46" s="8" t="s">
         <v>81</v>
       </c>
       <c r="O46" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="P46" s="10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="Q46" s="10" t="s">
         <v>37</v>
@@ -4568,42 +4595,42 @@
         <v>38</v>
       </c>
       <c r="S46" s="10" t="s">
-        <v>39</v>
+        <v>139</v>
       </c>
       <c r="T46" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U46" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="V46" s="10" t="s">
-        <v>373</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="C47" s="7" t="s">
+      <c r="E47" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="F47" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="G47" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="H47" s="7" t="s">
         <v>377</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>375</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>378</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>22</v>
@@ -4615,7 +4642,7 @@
         <v>31</v>
       </c>
       <c r="L47" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M47" s="7" t="s">
         <v>48</v>
@@ -4624,16 +4651,16 @@
         <v>81</v>
       </c>
       <c r="O47" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="P47" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="P47" s="7" t="s">
-        <v>381</v>
-      </c>
       <c r="Q47" s="7" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="R47" s="7" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="S47" s="7" t="s">
         <v>39</v>
@@ -4642,9 +4669,77 @@
         <v>40</v>
       </c>
       <c r="U47" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="V47" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="V47" s="7" t="s">
+    </row>
+    <row r="48" spans="1:22" ht="30" customHeight="1">
+      <c r="A48" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J48" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K48" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L48" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="M48" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="N48" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="O48" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="P48" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q48" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="R48" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="S48" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="T48" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="U48" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="V48" s="10" t="s">
         <v>256</v>
       </c>
     </row>
@@ -4695,7 +4790,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4719,55 +4814,55 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" s="2" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="F2" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="C3" s="2" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="2" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="2" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4775,16 +4870,16 @@
     </row>
     <row r="6" spans="1:22">
       <c r="C6" s="2" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="F6" s="3">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -4869,7 +4964,7 @@
         <v>110</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>112</v>
@@ -4884,10 +4979,10 @@
         <v>86</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>115</v>
@@ -4899,10 +4994,10 @@
         <v>196</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>52</v>
@@ -4914,7 +5009,7 @@
         <v>39</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="U9" s="7" t="s">
         <v>120</v>
@@ -4946,22 +5041,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>